<commit_message>
Dodanie podrozdzialu do sniezycy
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4132AD94-D596-4167-B949-6CF646184376}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F82C239-914B-4ECB-971A-539734C5A46D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,9 @@
     <sheet name="Baza danych - inicjacja pąków" sheetId="1" r:id="rId2"/>
     <sheet name="Baza danych - pasażowanie" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Baza danych - inicjacja pąków'!$A$1:$AQ$159</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1566,10 +1569,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1699,7 @@
       <c r="AP1" s="18"/>
       <c r="AQ1" s="18"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -14478,7 +14482,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>53</v>
       </c>
@@ -14607,7 +14611,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>53</v>
       </c>
@@ -14736,7 +14740,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>53</v>
       </c>
@@ -14865,7 +14869,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>53</v>
       </c>
@@ -14994,7 +14998,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>53</v>
       </c>
@@ -15123,7 +15127,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>53</v>
       </c>
@@ -15252,7 +15256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>53</v>
       </c>
@@ -15381,7 +15385,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>53</v>
       </c>
@@ -15510,7 +15514,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>53</v>
       </c>
@@ -15639,7 +15643,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>53</v>
       </c>
@@ -15768,7 +15772,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>53</v>
       </c>
@@ -15897,7 +15901,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>53</v>
       </c>
@@ -16026,7 +16030,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>53</v>
       </c>
@@ -16155,7 +16159,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>53</v>
       </c>
@@ -16284,7 +16288,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>53</v>
       </c>
@@ -16415,7 +16419,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>53</v>
       </c>
@@ -16546,7 +16550,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>53</v>
       </c>
@@ -16677,7 +16681,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>53</v>
       </c>
@@ -16808,7 +16812,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>53</v>
       </c>
@@ -16939,7 +16943,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>53</v>
       </c>
@@ -17070,7 +17074,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>53</v>
       </c>
@@ -17201,7 +17205,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>89</v>
       </c>
@@ -17330,7 +17334,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>89</v>
       </c>
@@ -17459,7 +17463,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>89</v>
       </c>
@@ -17588,7 +17592,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>89</v>
       </c>
@@ -17717,7 +17721,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>89</v>
       </c>
@@ -17846,7 +17850,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>89</v>
       </c>
@@ -17975,7 +17979,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>89</v>
       </c>
@@ -18104,7 +18108,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>89</v>
       </c>
@@ -18233,7 +18237,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>89</v>
       </c>
@@ -18362,7 +18366,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>89</v>
       </c>
@@ -18491,7 +18495,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>89</v>
       </c>
@@ -18620,7 +18624,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>89</v>
       </c>
@@ -18749,7 +18753,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>89</v>
       </c>
@@ -18878,7 +18882,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>89</v>
       </c>
@@ -19007,7 +19011,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>89</v>
       </c>
@@ -19136,7 +19140,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>89</v>
       </c>
@@ -19265,7 +19269,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>89</v>
       </c>
@@ -19394,7 +19398,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>89</v>
       </c>
@@ -19523,7 +19527,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>100</v>
       </c>
@@ -19652,7 +19656,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>100</v>
       </c>
@@ -19781,7 +19785,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>100</v>
       </c>
@@ -19910,7 +19914,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>100</v>
       </c>
@@ -20039,7 +20043,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>100</v>
       </c>
@@ -20168,7 +20172,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>100</v>
       </c>
@@ -20297,7 +20301,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>100</v>
       </c>
@@ -20426,7 +20430,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>100</v>
       </c>
@@ -20555,7 +20559,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>100</v>
       </c>
@@ -20684,7 +20688,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>100</v>
       </c>
@@ -20813,7 +20817,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="150" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>100</v>
       </c>
@@ -20942,7 +20946,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="151" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>100</v>
       </c>
@@ -21071,7 +21075,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="152" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>100</v>
       </c>
@@ -21200,7 +21204,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="153" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>100</v>
       </c>
@@ -21329,7 +21333,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="154" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>100</v>
       </c>
@@ -21458,7 +21462,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>100</v>
       </c>
@@ -21587,7 +21591,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="156" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>100</v>
       </c>
@@ -21716,7 +21720,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="157" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>100</v>
       </c>
@@ -21845,7 +21849,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="158" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>100</v>
       </c>
@@ -21974,7 +21978,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="159" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>100</v>
       </c>
@@ -22104,6 +22108,40 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AQ159" xr:uid="{A3EB1D5E-4AF2-4E96-A39F-D43A7CF18BB2}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Snieżyca karpacka"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="11" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="13" showButton="0"/>
+    <filterColumn colId="15" showButton="0"/>
+    <filterColumn colId="16" showButton="0"/>
+    <filterColumn colId="17" showButton="0"/>
+    <filterColumn colId="19" showButton="0"/>
+    <filterColumn colId="20" showButton="0"/>
+    <filterColumn colId="21" showButton="0"/>
+    <filterColumn colId="23" showButton="0"/>
+    <filterColumn colId="24" showButton="0"/>
+    <filterColumn colId="25" showButton="0"/>
+    <filterColumn colId="27" showButton="0"/>
+    <filterColumn colId="28" showButton="0"/>
+    <filterColumn colId="29" showButton="0"/>
+    <filterColumn colId="31" showButton="0"/>
+    <filterColumn colId="32" showButton="0"/>
+    <filterColumn colId="33" showButton="0"/>
+    <filterColumn colId="35" showButton="0"/>
+    <filterColumn colId="36" showButton="0"/>
+    <filterColumn colId="37" showButton="0"/>
+    <filterColumn colId="39" showButton="0"/>
+    <filterColumn colId="40" showButton="0"/>
+    <filterColumn colId="41" showButton="0"/>
+  </autoFilter>
   <mergeCells count="16">
     <mergeCell ref="AN1:AQ1"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Sniezyca koniec rozdzialu o inicjacji kultur
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE7324C-2472-496F-A423-5E64DCCC7B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9F3B3E-64A9-46B8-B7D8-EE64A2EBF95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeracja eksplantatów" sheetId="4" r:id="rId1"/>
     <sheet name="Baza danych - inicjacja pąków" sheetId="1" r:id="rId2"/>
-    <sheet name="Baza danych - pasażowanie" sheetId="3" r:id="rId3"/>
+    <sheet name="Baza danych - rozwoj i ukorz" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Baza danych - inicjacja pąków'!$A$1:$AQ$159</definedName>
@@ -1584,10 +1584,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A79" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1714,7 @@
       <c r="AP1" s="18"/>
       <c r="AQ1" s="18"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -14668,7 +14669,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>52</v>
       </c>
@@ -14797,7 +14798,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>52</v>
       </c>
@@ -14926,7 +14927,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>52</v>
       </c>
@@ -15055,7 +15056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>52</v>
       </c>
@@ -15184,7 +15185,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>52</v>
       </c>
@@ -15313,7 +15314,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>52</v>
       </c>
@@ -15442,7 +15443,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>52</v>
       </c>
@@ -15571,7 +15572,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>52</v>
       </c>
@@ -15700,7 +15701,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>52</v>
       </c>
@@ -15829,7 +15830,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>52</v>
       </c>
@@ -15958,7 +15959,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>52</v>
       </c>
@@ -16087,7 +16088,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>52</v>
       </c>
@@ -16216,7 +16217,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>52</v>
       </c>
@@ -16345,7 +16346,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>52</v>
       </c>
@@ -16474,7 +16475,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>52</v>
       </c>
@@ -16605,7 +16606,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>52</v>
       </c>
@@ -16736,7 +16737,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>52</v>
       </c>
@@ -16867,7 +16868,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>52</v>
       </c>
@@ -16998,7 +16999,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>52</v>
       </c>
@@ -17129,7 +17130,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>52</v>
       </c>
@@ -17260,7 +17261,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>52</v>
       </c>
@@ -17391,7 +17392,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>81</v>
       </c>
@@ -17520,7 +17521,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>81</v>
       </c>
@@ -17649,7 +17650,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>81</v>
       </c>
@@ -17778,7 +17779,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>81</v>
       </c>
@@ -17907,7 +17908,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>81</v>
       </c>
@@ -18036,7 +18037,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>81</v>
       </c>
@@ -18165,7 +18166,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>81</v>
       </c>
@@ -18294,7 +18295,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>81</v>
       </c>
@@ -18423,7 +18424,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>81</v>
       </c>
@@ -18552,7 +18553,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>81</v>
       </c>
@@ -18681,7 +18682,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>81</v>
       </c>
@@ -18810,7 +18811,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>81</v>
       </c>
@@ -18939,7 +18940,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>81</v>
       </c>
@@ -19068,7 +19069,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>81</v>
       </c>
@@ -19197,7 +19198,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>81</v>
       </c>
@@ -19326,7 +19327,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>81</v>
       </c>
@@ -19455,7 +19456,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>81</v>
       </c>
@@ -19584,7 +19585,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>81</v>
       </c>
@@ -19713,7 +19714,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>92</v>
       </c>
@@ -19842,7 +19843,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>92</v>
       </c>
@@ -19971,7 +19972,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>92</v>
       </c>
@@ -20100,7 +20101,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>92</v>
       </c>
@@ -20229,7 +20230,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>92</v>
       </c>
@@ -20358,7 +20359,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>92</v>
       </c>
@@ -20487,7 +20488,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>92</v>
       </c>
@@ -20616,7 +20617,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>92</v>
       </c>
@@ -20745,7 +20746,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>92</v>
       </c>
@@ -20874,7 +20875,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>92</v>
       </c>
@@ -21003,7 +21004,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>92</v>
       </c>
@@ -21132,7 +21133,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>92</v>
       </c>
@@ -21261,7 +21262,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>92</v>
       </c>
@@ -21390,7 +21391,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>92</v>
       </c>
@@ -21519,7 +21520,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>92</v>
       </c>
@@ -21648,7 +21649,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>92</v>
       </c>
@@ -21777,7 +21778,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>92</v>
       </c>
@@ -21906,7 +21907,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>92</v>
       </c>
@@ -22035,7 +22036,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="158" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>92</v>
       </c>
@@ -22164,7 +22165,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="159" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>92</v>
       </c>
@@ -22295,6 +22296,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AQ159" xr:uid="{A3EB1D5E-4AF2-4E96-A39F-D43A7CF18BB2}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Snieżyca karpacka"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
     <filterColumn colId="9" showButton="0"/>
@@ -22348,10 +22354,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:I4"/>
+  <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22410,6 +22416,206 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="4">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Zakonczenie rozdzialu o metodyce sniezyca - bez nadania pylku
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B17F7-2FCD-4B86-A7BF-D90BAA26F03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D25081-F9F3-44FB-8456-D55AB710635C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,6 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Baza danych - inicjacja pąków'!$A$1:$AQ$159</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Baza danych - rozwoj i ukorz'!$B$1:$I$290</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -875,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -923,6 +924,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -22354,48 +22358,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:I291"/>
+  <dimension ref="B1:I290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H285" sqref="H285"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="4" width="23.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>107</v>
-      </c>
+      <c r="E2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -22405,7 +22432,7 @@
         <v>109</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>110</v>
@@ -22427,7 +22454,7 @@
         <v>109</v>
       </c>
       <c r="D4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>110</v>
@@ -22449,7 +22476,7 @@
         <v>109</v>
       </c>
       <c r="D5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>110</v>
@@ -22471,7 +22498,7 @@
         <v>109</v>
       </c>
       <c r="D6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>110</v>
@@ -22493,7 +22520,7 @@
         <v>109</v>
       </c>
       <c r="D7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>110</v>
@@ -22515,7 +22542,7 @@
         <v>109</v>
       </c>
       <c r="D8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>110</v>
@@ -22537,7 +22564,7 @@
         <v>109</v>
       </c>
       <c r="D9" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>110</v>
@@ -22559,7 +22586,7 @@
         <v>109</v>
       </c>
       <c r="D10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>110</v>
@@ -22581,7 +22608,7 @@
         <v>109</v>
       </c>
       <c r="D11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>110</v>
@@ -22603,7 +22630,7 @@
         <v>109</v>
       </c>
       <c r="D12" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>110</v>
@@ -22625,7 +22652,7 @@
         <v>109</v>
       </c>
       <c r="D13" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>110</v>
@@ -22634,7 +22661,7 @@
         <v>51</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
@@ -22647,7 +22674,7 @@
         <v>109</v>
       </c>
       <c r="D14" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>110</v>
@@ -22669,7 +22696,7 @@
         <v>109</v>
       </c>
       <c r="D15" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>110</v>
@@ -22691,7 +22718,7 @@
         <v>109</v>
       </c>
       <c r="D16" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>110</v>
@@ -22713,7 +22740,7 @@
         <v>109</v>
       </c>
       <c r="D17" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>110</v>
@@ -22735,7 +22762,7 @@
         <v>109</v>
       </c>
       <c r="D18" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>110</v>
@@ -22757,7 +22784,7 @@
         <v>109</v>
       </c>
       <c r="D19" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>110</v>
@@ -22779,7 +22806,7 @@
         <v>109</v>
       </c>
       <c r="D20" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>110</v>
@@ -22801,7 +22828,7 @@
         <v>109</v>
       </c>
       <c r="D21" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>110</v>
@@ -22823,7 +22850,7 @@
         <v>109</v>
       </c>
       <c r="D22" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>110</v>
@@ -22845,13 +22872,13 @@
         <v>109</v>
       </c>
       <c r="D23" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>51</v>
+      <c r="F23" s="12">
+        <v>43196</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>26</v>
@@ -22867,16 +22894,16 @@
         <v>109</v>
       </c>
       <c r="D24" s="4">
+        <v>23</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="12">
+        <v>43210</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" s="12">
-        <v>43196</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
@@ -22889,7 +22916,7 @@
         <v>109</v>
       </c>
       <c r="D25" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>110</v>
@@ -22911,7 +22938,7 @@
         <v>109</v>
       </c>
       <c r="D26" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>110</v>
@@ -22933,7 +22960,7 @@
         <v>109</v>
       </c>
       <c r="D27" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>110</v>
@@ -22955,7 +22982,7 @@
         <v>109</v>
       </c>
       <c r="D28" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>110</v>
@@ -22977,7 +23004,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>110</v>
@@ -22999,7 +23026,7 @@
         <v>109</v>
       </c>
       <c r="D30" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>110</v>
@@ -23021,7 +23048,7 @@
         <v>109</v>
       </c>
       <c r="D31" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>110</v>
@@ -23043,7 +23070,7 @@
         <v>109</v>
       </c>
       <c r="D32" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>110</v>
@@ -23065,16 +23092,16 @@
         <v>109</v>
       </c>
       <c r="D33" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F33" s="12">
-        <v>43210</v>
+        <v>43168</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="6"/>
@@ -23087,7 +23114,7 @@
         <v>109</v>
       </c>
       <c r="D34" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>110</v>
@@ -23109,7 +23136,7 @@
         <v>109</v>
       </c>
       <c r="D35" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>110</v>
@@ -23131,7 +23158,7 @@
         <v>109</v>
       </c>
       <c r="D36" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>110</v>
@@ -23153,18 +23180,18 @@
         <v>109</v>
       </c>
       <c r="D37" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F37" s="12">
-        <v>43168</v>
+        <v>43175</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="H37" s="4"/>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -23175,7 +23202,7 @@
         <v>109</v>
       </c>
       <c r="D38" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>110</v>
@@ -23197,7 +23224,7 @@
         <v>109</v>
       </c>
       <c r="D39" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>110</v>
@@ -23219,16 +23246,16 @@
         <v>109</v>
       </c>
       <c r="D40" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F40" s="12">
-        <v>43175</v>
+        <v>43206</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="6"/>
@@ -23241,7 +23268,7 @@
         <v>109</v>
       </c>
       <c r="D41" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>110</v>
@@ -23263,7 +23290,7 @@
         <v>109</v>
       </c>
       <c r="D42" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>110</v>
@@ -23285,7 +23312,7 @@
         <v>109</v>
       </c>
       <c r="D43" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>110</v>
@@ -23307,7 +23334,7 @@
         <v>109</v>
       </c>
       <c r="D44" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>110</v>
@@ -23329,7 +23356,7 @@
         <v>109</v>
       </c>
       <c r="D45" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>110</v>
@@ -23351,7 +23378,7 @@
         <v>109</v>
       </c>
       <c r="D46" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>110</v>
@@ -23373,7 +23400,7 @@
         <v>109</v>
       </c>
       <c r="D47" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>110</v>
@@ -23395,7 +23422,7 @@
         <v>109</v>
       </c>
       <c r="D48" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>110</v>
@@ -23417,7 +23444,7 @@
         <v>109</v>
       </c>
       <c r="D49" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>110</v>
@@ -23439,7 +23466,7 @@
         <v>109</v>
       </c>
       <c r="D50" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>110</v>
@@ -23461,7 +23488,7 @@
         <v>109</v>
       </c>
       <c r="D51" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>110</v>
@@ -23483,7 +23510,7 @@
         <v>109</v>
       </c>
       <c r="D52" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>110</v>
@@ -23505,7 +23532,7 @@
         <v>109</v>
       </c>
       <c r="D53" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>110</v>
@@ -23527,7 +23554,7 @@
         <v>109</v>
       </c>
       <c r="D54" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>110</v>
@@ -23549,16 +23576,16 @@
         <v>109</v>
       </c>
       <c r="D55" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F55" s="12">
-        <v>43206</v>
+        <v>43182</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="6"/>
@@ -23571,7 +23598,7 @@
         <v>109</v>
       </c>
       <c r="D56" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>110</v>
@@ -23593,7 +23620,7 @@
         <v>109</v>
       </c>
       <c r="D57" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>110</v>
@@ -23615,7 +23642,7 @@
         <v>109</v>
       </c>
       <c r="D58" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>110</v>
@@ -23637,7 +23664,7 @@
         <v>109</v>
       </c>
       <c r="D59" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>110</v>
@@ -23659,7 +23686,7 @@
         <v>109</v>
       </c>
       <c r="D60" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>110</v>
@@ -23681,7 +23708,7 @@
         <v>109</v>
       </c>
       <c r="D61" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>110</v>
@@ -23703,7 +23730,7 @@
         <v>109</v>
       </c>
       <c r="D62" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>110</v>
@@ -23725,7 +23752,7 @@
         <v>109</v>
       </c>
       <c r="D63" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>110</v>
@@ -23747,7 +23774,7 @@
         <v>109</v>
       </c>
       <c r="D64" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>110</v>
@@ -23769,7 +23796,7 @@
         <v>109</v>
       </c>
       <c r="D65" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>110</v>
@@ -23778,7 +23805,7 @@
         <v>43182</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="6"/>
@@ -23791,7 +23818,7 @@
         <v>109</v>
       </c>
       <c r="D66" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>110</v>
@@ -23813,7 +23840,7 @@
         <v>109</v>
       </c>
       <c r="D67" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>110</v>
@@ -23835,7 +23862,7 @@
         <v>109</v>
       </c>
       <c r="D68" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>110</v>
@@ -23857,16 +23884,16 @@
         <v>109</v>
       </c>
       <c r="D69" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F69" s="12">
-        <v>43182</v>
+        <v>43175</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="6"/>
@@ -23879,7 +23906,7 @@
         <v>109</v>
       </c>
       <c r="D70" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>110</v>
@@ -23901,7 +23928,7 @@
         <v>109</v>
       </c>
       <c r="D71" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>110</v>
@@ -23923,7 +23950,7 @@
         <v>109</v>
       </c>
       <c r="D72" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>110</v>
@@ -23945,7 +23972,7 @@
         <v>109</v>
       </c>
       <c r="D73" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>110</v>
@@ -23954,7 +23981,7 @@
         <v>43175</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="6"/>
@@ -23967,7 +23994,7 @@
         <v>109</v>
       </c>
       <c r="D74" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>110</v>
@@ -23989,7 +24016,7 @@
         <v>109</v>
       </c>
       <c r="D75" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>110</v>
@@ -24011,7 +24038,7 @@
         <v>109</v>
       </c>
       <c r="D76" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>110</v>
@@ -24033,7 +24060,7 @@
         <v>109</v>
       </c>
       <c r="D77" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>110</v>
@@ -24055,7 +24082,7 @@
         <v>109</v>
       </c>
       <c r="D78" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>110</v>
@@ -24077,7 +24104,7 @@
         <v>109</v>
       </c>
       <c r="D79" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>110</v>
@@ -24099,16 +24126,16 @@
         <v>109</v>
       </c>
       <c r="D80" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F80" s="12">
-        <v>43175</v>
+        <v>43182</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="6"/>
@@ -24121,16 +24148,16 @@
         <v>109</v>
       </c>
       <c r="D81" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F81" s="12">
-        <v>43182</v>
+        <v>43196</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="6"/>
@@ -24143,7 +24170,7 @@
         <v>109</v>
       </c>
       <c r="D82" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>110</v>
@@ -24165,7 +24192,7 @@
         <v>109</v>
       </c>
       <c r="D83" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>110</v>
@@ -24187,7 +24214,7 @@
         <v>109</v>
       </c>
       <c r="D84" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>110</v>
@@ -24209,7 +24236,7 @@
         <v>109</v>
       </c>
       <c r="D85" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>110</v>
@@ -24231,7 +24258,7 @@
         <v>109</v>
       </c>
       <c r="D86" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>110</v>
@@ -24253,7 +24280,7 @@
         <v>109</v>
       </c>
       <c r="D87" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>110</v>
@@ -24275,7 +24302,7 @@
         <v>109</v>
       </c>
       <c r="D88" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>110</v>
@@ -24297,7 +24324,7 @@
         <v>109</v>
       </c>
       <c r="D89" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>110</v>
@@ -24319,7 +24346,7 @@
         <v>109</v>
       </c>
       <c r="D90" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>110</v>
@@ -24341,7 +24368,7 @@
         <v>109</v>
       </c>
       <c r="D91" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>110</v>
@@ -24363,7 +24390,7 @@
         <v>109</v>
       </c>
       <c r="D92" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>110</v>
@@ -24385,7 +24412,7 @@
         <v>109</v>
       </c>
       <c r="D93" s="4">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>110</v>
@@ -24407,7 +24434,7 @@
         <v>109</v>
       </c>
       <c r="D94" s="4">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>110</v>
@@ -24429,7 +24456,7 @@
         <v>109</v>
       </c>
       <c r="D95" s="4">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>110</v>
@@ -24451,16 +24478,16 @@
         <v>109</v>
       </c>
       <c r="D96" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F96" s="12">
-        <v>43196</v>
+        <v>43175</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H96" s="4"/>
       <c r="I96" s="6"/>
@@ -24473,7 +24500,7 @@
         <v>109</v>
       </c>
       <c r="D97" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>110</v>
@@ -24495,7 +24522,7 @@
         <v>109</v>
       </c>
       <c r="D98" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>110</v>
@@ -24517,7 +24544,7 @@
         <v>109</v>
       </c>
       <c r="D99" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>110</v>
@@ -24539,7 +24566,7 @@
         <v>109</v>
       </c>
       <c r="D100" s="4">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>110</v>
@@ -24561,16 +24588,16 @@
         <v>109</v>
       </c>
       <c r="D101" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F101" s="12">
-        <v>43175</v>
+        <v>43196</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="6"/>
@@ -24583,13 +24610,13 @@
         <v>109</v>
       </c>
       <c r="D102" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F102" s="12">
-        <v>43196</v>
+        <v>43182</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>24</v>
@@ -24605,7 +24632,7 @@
         <v>109</v>
       </c>
       <c r="D103" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>110</v>
@@ -24627,7 +24654,7 @@
         <v>109</v>
       </c>
       <c r="D104" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>110</v>
@@ -24649,16 +24676,16 @@
         <v>109</v>
       </c>
       <c r="D105" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F105" s="12">
-        <v>43182</v>
+        <v>43196</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H105" s="4"/>
       <c r="I105" s="6"/>
@@ -24671,7 +24698,7 @@
         <v>109</v>
       </c>
       <c r="D106" s="4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>110</v>
@@ -24693,7 +24720,7 @@
         <v>109</v>
       </c>
       <c r="D107" s="4">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>110</v>
@@ -24715,7 +24742,7 @@
         <v>109</v>
       </c>
       <c r="D108" s="4">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>110</v>
@@ -24737,7 +24764,7 @@
         <v>109</v>
       </c>
       <c r="D109" s="4">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>110</v>
@@ -24759,7 +24786,7 @@
         <v>109</v>
       </c>
       <c r="D110" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>110</v>
@@ -24781,7 +24808,7 @@
         <v>109</v>
       </c>
       <c r="D111" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>110</v>
@@ -24803,16 +24830,16 @@
         <v>109</v>
       </c>
       <c r="D112" s="4">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F112" s="12">
-        <v>43196</v>
+        <v>43206</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H112" s="4"/>
       <c r="I112" s="6"/>
@@ -24825,7 +24852,7 @@
         <v>109</v>
       </c>
       <c r="D113" s="4">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>110</v>
@@ -24847,7 +24874,7 @@
         <v>109</v>
       </c>
       <c r="D114" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>110</v>
@@ -24869,7 +24896,7 @@
         <v>109</v>
       </c>
       <c r="D115" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>110</v>
@@ -24884,23 +24911,23 @@
       <c r="I115" s="6"/>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
-        <v>108</v>
+      <c r="B116" s="12">
+        <v>43273</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="D116" s="4">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F116" s="12">
-        <v>43206</v>
+        <v>43231</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="6"/>
@@ -24913,7 +24940,7 @@
         <v>53</v>
       </c>
       <c r="D117" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>110</v>
@@ -24935,7 +24962,7 @@
         <v>53</v>
       </c>
       <c r="D118" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>110</v>
@@ -24957,7 +24984,7 @@
         <v>53</v>
       </c>
       <c r="D119" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>110</v>
@@ -24979,7 +25006,7 @@
         <v>53</v>
       </c>
       <c r="D120" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>110</v>
@@ -25001,7 +25028,7 @@
         <v>53</v>
       </c>
       <c r="D121" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>110</v>
@@ -25023,7 +25050,7 @@
         <v>53</v>
       </c>
       <c r="D122" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E122" s="4" t="s">
         <v>110</v>
@@ -25045,7 +25072,7 @@
         <v>53</v>
       </c>
       <c r="D123" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>110</v>
@@ -25067,7 +25094,7 @@
         <v>53</v>
       </c>
       <c r="D124" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>110</v>
@@ -25089,7 +25116,7 @@
         <v>53</v>
       </c>
       <c r="D125" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>110</v>
@@ -25111,7 +25138,7 @@
         <v>53</v>
       </c>
       <c r="D126" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>110</v>
@@ -25133,7 +25160,7 @@
         <v>53</v>
       </c>
       <c r="D127" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>110</v>
@@ -25155,7 +25182,7 @@
         <v>53</v>
       </c>
       <c r="D128" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E128" s="4" t="s">
         <v>110</v>
@@ -25177,7 +25204,7 @@
         <v>53</v>
       </c>
       <c r="D129" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>110</v>
@@ -25199,7 +25226,7 @@
         <v>53</v>
       </c>
       <c r="D130" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>110</v>
@@ -25221,7 +25248,7 @@
         <v>53</v>
       </c>
       <c r="D131" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>110</v>
@@ -25243,7 +25270,7 @@
         <v>53</v>
       </c>
       <c r="D132" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E132" s="4" t="s">
         <v>110</v>
@@ -25265,7 +25292,7 @@
         <v>53</v>
       </c>
       <c r="D133" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>110</v>
@@ -25287,7 +25314,7 @@
         <v>53</v>
       </c>
       <c r="D134" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>110</v>
@@ -25309,7 +25336,7 @@
         <v>53</v>
       </c>
       <c r="D135" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>110</v>
@@ -25331,7 +25358,7 @@
         <v>53</v>
       </c>
       <c r="D136" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>110</v>
@@ -25353,7 +25380,7 @@
         <v>53</v>
       </c>
       <c r="D137" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>110</v>
@@ -25375,7 +25402,7 @@
         <v>53</v>
       </c>
       <c r="D138" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>110</v>
@@ -25397,7 +25424,7 @@
         <v>53</v>
       </c>
       <c r="D139" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>110</v>
@@ -25419,7 +25446,7 @@
         <v>53</v>
       </c>
       <c r="D140" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>110</v>
@@ -25428,7 +25455,7 @@
         <v>43231</v>
       </c>
       <c r="G140" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="6"/>
@@ -25441,7 +25468,7 @@
         <v>53</v>
       </c>
       <c r="D141" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E141" s="4" t="s">
         <v>110</v>
@@ -25463,7 +25490,7 @@
         <v>53</v>
       </c>
       <c r="D142" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E142" s="4" t="s">
         <v>110</v>
@@ -25485,7 +25512,7 @@
         <v>53</v>
       </c>
       <c r="D143" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>110</v>
@@ -25507,7 +25534,7 @@
         <v>53</v>
       </c>
       <c r="D144" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>110</v>
@@ -25529,7 +25556,7 @@
         <v>53</v>
       </c>
       <c r="D145" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>110</v>
@@ -25551,7 +25578,7 @@
         <v>53</v>
       </c>
       <c r="D146" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>110</v>
@@ -25573,7 +25600,7 @@
         <v>53</v>
       </c>
       <c r="D147" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>110</v>
@@ -25595,7 +25622,7 @@
         <v>53</v>
       </c>
       <c r="D148" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>110</v>
@@ -25617,7 +25644,7 @@
         <v>53</v>
       </c>
       <c r="D149" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E149" s="4" t="s">
         <v>110</v>
@@ -25639,7 +25666,7 @@
         <v>53</v>
       </c>
       <c r="D150" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>110</v>
@@ -25661,7 +25688,7 @@
         <v>53</v>
       </c>
       <c r="D151" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>110</v>
@@ -25683,7 +25710,7 @@
         <v>53</v>
       </c>
       <c r="D152" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>110</v>
@@ -25705,7 +25732,7 @@
         <v>53</v>
       </c>
       <c r="D153" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>110</v>
@@ -25727,7 +25754,7 @@
         <v>53</v>
       </c>
       <c r="D154" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>110</v>
@@ -25749,7 +25776,7 @@
         <v>53</v>
       </c>
       <c r="D155" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>110</v>
@@ -25771,7 +25798,7 @@
         <v>53</v>
       </c>
       <c r="D156" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E156" s="4" t="s">
         <v>110</v>
@@ -25793,7 +25820,7 @@
         <v>53</v>
       </c>
       <c r="D157" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E157" s="4" t="s">
         <v>110</v>
@@ -25815,7 +25842,7 @@
         <v>53</v>
       </c>
       <c r="D158" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E158" s="4" t="s">
         <v>110</v>
@@ -25837,7 +25864,7 @@
         <v>53</v>
       </c>
       <c r="D159" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E159" s="4" t="s">
         <v>110</v>
@@ -25859,7 +25886,7 @@
         <v>53</v>
       </c>
       <c r="D160" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E160" s="4" t="s">
         <v>110</v>
@@ -25881,7 +25908,7 @@
         <v>53</v>
       </c>
       <c r="D161" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>110</v>
@@ -25903,7 +25930,7 @@
         <v>53</v>
       </c>
       <c r="D162" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E162" s="4" t="s">
         <v>110</v>
@@ -25925,7 +25952,7 @@
         <v>53</v>
       </c>
       <c r="D163" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>110</v>
@@ -25947,7 +25974,7 @@
         <v>53</v>
       </c>
       <c r="D164" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E164" s="4" t="s">
         <v>110</v>
@@ -25969,7 +25996,7 @@
         <v>53</v>
       </c>
       <c r="D165" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E165" s="4" t="s">
         <v>110</v>
@@ -25991,7 +26018,7 @@
         <v>53</v>
       </c>
       <c r="D166" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E166" s="4" t="s">
         <v>110</v>
@@ -26013,7 +26040,7 @@
         <v>53</v>
       </c>
       <c r="D167" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>110</v>
@@ -26022,7 +26049,7 @@
         <v>43231</v>
       </c>
       <c r="G167" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H167" s="4"/>
       <c r="I167" s="6"/>
@@ -26035,7 +26062,7 @@
         <v>53</v>
       </c>
       <c r="D168" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E168" s="4" t="s">
         <v>110</v>
@@ -26057,7 +26084,7 @@
         <v>53</v>
       </c>
       <c r="D169" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E169" s="4" t="s">
         <v>110</v>
@@ -26079,7 +26106,7 @@
         <v>53</v>
       </c>
       <c r="D170" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E170" s="4" t="s">
         <v>110</v>
@@ -26101,7 +26128,7 @@
         <v>53</v>
       </c>
       <c r="D171" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E171" s="4" t="s">
         <v>110</v>
@@ -26123,7 +26150,7 @@
         <v>53</v>
       </c>
       <c r="D172" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E172" s="4" t="s">
         <v>110</v>
@@ -26145,7 +26172,7 @@
         <v>53</v>
       </c>
       <c r="D173" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E173" s="4" t="s">
         <v>110</v>
@@ -26167,7 +26194,7 @@
         <v>53</v>
       </c>
       <c r="D174" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E174" s="4" t="s">
         <v>110</v>
@@ -26189,16 +26216,16 @@
         <v>53</v>
       </c>
       <c r="D175" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E175" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F175" s="12">
-        <v>43231</v>
+        <v>43217</v>
       </c>
       <c r="G175" s="4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H175" s="4"/>
       <c r="I175" s="6"/>
@@ -26211,7 +26238,7 @@
         <v>53</v>
       </c>
       <c r="D176" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E176" s="4" t="s">
         <v>110</v>
@@ -26233,7 +26260,7 @@
         <v>53</v>
       </c>
       <c r="D177" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E177" s="4" t="s">
         <v>110</v>
@@ -26255,7 +26282,7 @@
         <v>53</v>
       </c>
       <c r="D178" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E178" s="4" t="s">
         <v>110</v>
@@ -26277,7 +26304,7 @@
         <v>53</v>
       </c>
       <c r="D179" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E179" s="4" t="s">
         <v>110</v>
@@ -26299,7 +26326,7 @@
         <v>53</v>
       </c>
       <c r="D180" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E180" s="4" t="s">
         <v>110</v>
@@ -26321,7 +26348,7 @@
         <v>53</v>
       </c>
       <c r="D181" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E181" s="4" t="s">
         <v>110</v>
@@ -26343,7 +26370,7 @@
         <v>53</v>
       </c>
       <c r="D182" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E182" s="4" t="s">
         <v>110</v>
@@ -26365,7 +26392,7 @@
         <v>53</v>
       </c>
       <c r="D183" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E183" s="4" t="s">
         <v>110</v>
@@ -26387,7 +26414,7 @@
         <v>53</v>
       </c>
       <c r="D184" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E184" s="4" t="s">
         <v>110</v>
@@ -26409,7 +26436,7 @@
         <v>53</v>
       </c>
       <c r="D185" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E185" s="4" t="s">
         <v>110</v>
@@ -26431,7 +26458,7 @@
         <v>53</v>
       </c>
       <c r="D186" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E186" s="4" t="s">
         <v>110</v>
@@ -26453,7 +26480,7 @@
         <v>53</v>
       </c>
       <c r="D187" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E187" s="4" t="s">
         <v>110</v>
@@ -26475,7 +26502,7 @@
         <v>53</v>
       </c>
       <c r="D188" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E188" s="4" t="s">
         <v>110</v>
@@ -26497,7 +26524,7 @@
         <v>53</v>
       </c>
       <c r="D189" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E189" s="4" t="s">
         <v>110</v>
@@ -26519,7 +26546,7 @@
         <v>53</v>
       </c>
       <c r="D190" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E190" s="4" t="s">
         <v>110</v>
@@ -26541,7 +26568,7 @@
         <v>53</v>
       </c>
       <c r="D191" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E191" s="4" t="s">
         <v>110</v>
@@ -26563,7 +26590,7 @@
         <v>53</v>
       </c>
       <c r="D192" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E192" s="4" t="s">
         <v>110</v>
@@ -26572,7 +26599,7 @@
         <v>43217</v>
       </c>
       <c r="G192" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H192" s="4"/>
       <c r="I192" s="6"/>
@@ -26585,7 +26612,7 @@
         <v>53</v>
       </c>
       <c r="D193" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E193" s="4" t="s">
         <v>110</v>
@@ -26607,7 +26634,7 @@
         <v>53</v>
       </c>
       <c r="D194" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E194" s="4" t="s">
         <v>110</v>
@@ -26629,7 +26656,7 @@
         <v>53</v>
       </c>
       <c r="D195" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E195" s="4" t="s">
         <v>110</v>
@@ -26651,7 +26678,7 @@
         <v>53</v>
       </c>
       <c r="D196" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E196" s="4" t="s">
         <v>110</v>
@@ -26673,7 +26700,7 @@
         <v>53</v>
       </c>
       <c r="D197" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E197" s="4" t="s">
         <v>110</v>
@@ -26695,7 +26722,7 @@
         <v>53</v>
       </c>
       <c r="D198" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E198" s="4" t="s">
         <v>110</v>
@@ -26717,7 +26744,7 @@
         <v>53</v>
       </c>
       <c r="D199" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E199" s="4" t="s">
         <v>110</v>
@@ -26739,7 +26766,7 @@
         <v>53</v>
       </c>
       <c r="D200" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E200" s="4" t="s">
         <v>110</v>
@@ -26761,7 +26788,7 @@
         <v>53</v>
       </c>
       <c r="D201" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E201" s="4" t="s">
         <v>110</v>
@@ -26783,7 +26810,7 @@
         <v>53</v>
       </c>
       <c r="D202" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E202" s="4" t="s">
         <v>110</v>
@@ -26805,7 +26832,7 @@
         <v>53</v>
       </c>
       <c r="D203" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E203" s="4" t="s">
         <v>110</v>
@@ -26827,7 +26854,7 @@
         <v>53</v>
       </c>
       <c r="D204" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E204" s="4" t="s">
         <v>110</v>
@@ -26849,7 +26876,7 @@
         <v>53</v>
       </c>
       <c r="D205" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E205" s="4" t="s">
         <v>110</v>
@@ -26871,7 +26898,7 @@
         <v>53</v>
       </c>
       <c r="D206" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E206" s="4" t="s">
         <v>110</v>
@@ -26893,7 +26920,7 @@
         <v>53</v>
       </c>
       <c r="D207" s="4">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E207" s="4" t="s">
         <v>110</v>
@@ -26915,7 +26942,7 @@
         <v>53</v>
       </c>
       <c r="D208" s="4">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E208" s="4" t="s">
         <v>110</v>
@@ -26937,7 +26964,7 @@
         <v>53</v>
       </c>
       <c r="D209" s="4">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E209" s="4" t="s">
         <v>110</v>
@@ -26959,7 +26986,7 @@
         <v>53</v>
       </c>
       <c r="D210" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E210" s="4" t="s">
         <v>110</v>
@@ -26981,7 +27008,7 @@
         <v>53</v>
       </c>
       <c r="D211" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E211" s="4" t="s">
         <v>110</v>
@@ -27003,7 +27030,7 @@
         <v>53</v>
       </c>
       <c r="D212" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E212" s="4" t="s">
         <v>110</v>
@@ -27025,7 +27052,7 @@
         <v>53</v>
       </c>
       <c r="D213" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E213" s="4" t="s">
         <v>110</v>
@@ -27047,7 +27074,7 @@
         <v>53</v>
       </c>
       <c r="D214" s="4">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E214" s="4" t="s">
         <v>110</v>
@@ -27069,7 +27096,7 @@
         <v>53</v>
       </c>
       <c r="D215" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E215" s="4" t="s">
         <v>110</v>
@@ -27091,7 +27118,7 @@
         <v>53</v>
       </c>
       <c r="D216" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E216" s="4" t="s">
         <v>110</v>
@@ -27113,7 +27140,7 @@
         <v>53</v>
       </c>
       <c r="D217" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E217" s="4" t="s">
         <v>110</v>
@@ -27135,7 +27162,7 @@
         <v>53</v>
       </c>
       <c r="D218" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E218" s="4" t="s">
         <v>110</v>
@@ -27157,7 +27184,7 @@
         <v>53</v>
       </c>
       <c r="D219" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E219" s="4" t="s">
         <v>110</v>
@@ -27179,7 +27206,7 @@
         <v>53</v>
       </c>
       <c r="D220" s="4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E220" s="4" t="s">
         <v>110</v>
@@ -27201,7 +27228,7 @@
         <v>53</v>
       </c>
       <c r="D221" s="4">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E221" s="4" t="s">
         <v>110</v>
@@ -27223,7 +27250,7 @@
         <v>53</v>
       </c>
       <c r="D222" s="4">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E222" s="4" t="s">
         <v>110</v>
@@ -27245,7 +27272,7 @@
         <v>53</v>
       </c>
       <c r="D223" s="4">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E223" s="4" t="s">
         <v>110</v>
@@ -27267,7 +27294,7 @@
         <v>53</v>
       </c>
       <c r="D224" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E224" s="4" t="s">
         <v>110</v>
@@ -27289,7 +27316,7 @@
         <v>53</v>
       </c>
       <c r="D225" s="4">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E225" s="4" t="s">
         <v>110</v>
@@ -27311,7 +27338,7 @@
         <v>53</v>
       </c>
       <c r="D226" s="4">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E226" s="4" t="s">
         <v>110</v>
@@ -27333,7 +27360,7 @@
         <v>53</v>
       </c>
       <c r="D227" s="4">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E227" s="4" t="s">
         <v>110</v>
@@ -27355,7 +27382,7 @@
         <v>53</v>
       </c>
       <c r="D228" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E228" s="4" t="s">
         <v>110</v>
@@ -27377,7 +27404,7 @@
         <v>53</v>
       </c>
       <c r="D229" s="4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E229" s="4" t="s">
         <v>110</v>
@@ -27399,7 +27426,7 @@
         <v>53</v>
       </c>
       <c r="D230" s="4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E230" s="4" t="s">
         <v>110</v>
@@ -27421,7 +27448,7 @@
         <v>53</v>
       </c>
       <c r="D231" s="4">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E231" s="4" t="s">
         <v>110</v>
@@ -27443,7 +27470,7 @@
         <v>53</v>
       </c>
       <c r="D232" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E232" s="4" t="s">
         <v>110</v>
@@ -27465,7 +27492,7 @@
         <v>53</v>
       </c>
       <c r="D233" s="4">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E233" s="4" t="s">
         <v>110</v>
@@ -27487,7 +27514,7 @@
         <v>53</v>
       </c>
       <c r="D234" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E234" s="4" t="s">
         <v>110</v>
@@ -27509,16 +27536,16 @@
         <v>53</v>
       </c>
       <c r="D235" s="4">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E235" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F235" s="12">
-        <v>43217</v>
+        <v>43206</v>
       </c>
       <c r="G235" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="H235" s="4"/>
       <c r="I235" s="6"/>
@@ -27531,7 +27558,7 @@
         <v>53</v>
       </c>
       <c r="D236" s="4">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E236" s="4" t="s">
         <v>110</v>
@@ -27553,7 +27580,7 @@
         <v>53</v>
       </c>
       <c r="D237" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E237" s="4" t="s">
         <v>110</v>
@@ -27575,7 +27602,7 @@
         <v>53</v>
       </c>
       <c r="D238" s="4">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E238" s="4" t="s">
         <v>110</v>
@@ -27597,7 +27624,7 @@
         <v>53</v>
       </c>
       <c r="D239" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E239" s="4" t="s">
         <v>110</v>
@@ -27619,7 +27646,7 @@
         <v>53</v>
       </c>
       <c r="D240" s="4">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E240" s="4" t="s">
         <v>110</v>
@@ -27641,7 +27668,7 @@
         <v>53</v>
       </c>
       <c r="D241" s="4">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E241" s="4" t="s">
         <v>110</v>
@@ -27663,7 +27690,7 @@
         <v>53</v>
       </c>
       <c r="D242" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E242" s="4" t="s">
         <v>110</v>
@@ -27685,7 +27712,7 @@
         <v>53</v>
       </c>
       <c r="D243" s="4">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E243" s="4" t="s">
         <v>110</v>
@@ -27707,7 +27734,7 @@
         <v>53</v>
       </c>
       <c r="D244" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E244" s="4" t="s">
         <v>110</v>
@@ -27729,7 +27756,7 @@
         <v>53</v>
       </c>
       <c r="D245" s="4">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E245" s="4" t="s">
         <v>110</v>
@@ -27751,7 +27778,7 @@
         <v>53</v>
       </c>
       <c r="D246" s="4">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E246" s="4" t="s">
         <v>110</v>
@@ -27773,7 +27800,7 @@
         <v>53</v>
       </c>
       <c r="D247" s="4">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E247" s="4" t="s">
         <v>110</v>
@@ -27795,7 +27822,7 @@
         <v>53</v>
       </c>
       <c r="D248" s="4">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E248" s="4" t="s">
         <v>110</v>
@@ -27817,7 +27844,7 @@
         <v>53</v>
       </c>
       <c r="D249" s="4">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E249" s="4" t="s">
         <v>110</v>
@@ -27839,16 +27866,16 @@
         <v>53</v>
       </c>
       <c r="D250" s="4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E250" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F250" s="12">
-        <v>43206</v>
+        <v>43217</v>
       </c>
       <c r="G250" s="4" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="H250" s="4"/>
       <c r="I250" s="6"/>
@@ -27861,7 +27888,7 @@
         <v>53</v>
       </c>
       <c r="D251" s="4">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E251" s="4" t="s">
         <v>110</v>
@@ -27883,7 +27910,7 @@
         <v>53</v>
       </c>
       <c r="D252" s="4">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E252" s="4" t="s">
         <v>110</v>
@@ -27905,7 +27932,7 @@
         <v>53</v>
       </c>
       <c r="D253" s="4">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E253" s="4" t="s">
         <v>110</v>
@@ -27927,7 +27954,7 @@
         <v>53</v>
       </c>
       <c r="D254" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E254" s="4" t="s">
         <v>110</v>
@@ -27949,16 +27976,16 @@
         <v>53</v>
       </c>
       <c r="D255" s="4">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E255" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F255" s="12">
-        <v>43217</v>
+        <v>43206</v>
       </c>
       <c r="G255" s="4" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="H255" s="4"/>
       <c r="I255" s="6"/>
@@ -27971,7 +27998,7 @@
         <v>53</v>
       </c>
       <c r="D256" s="4">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E256" s="4" t="s">
         <v>110</v>
@@ -27993,7 +28020,7 @@
         <v>53</v>
       </c>
       <c r="D257" s="4">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E257" s="4" t="s">
         <v>110</v>
@@ -28015,7 +28042,7 @@
         <v>53</v>
       </c>
       <c r="D258" s="4">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E258" s="4" t="s">
         <v>110</v>
@@ -28037,7 +28064,7 @@
         <v>53</v>
       </c>
       <c r="D259" s="4">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E259" s="4" t="s">
         <v>110</v>
@@ -28059,7 +28086,7 @@
         <v>53</v>
       </c>
       <c r="D260" s="4">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E260" s="4" t="s">
         <v>110</v>
@@ -28081,7 +28108,7 @@
         <v>53</v>
       </c>
       <c r="D261" s="4">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E261" s="4" t="s">
         <v>110</v>
@@ -28103,7 +28130,7 @@
         <v>53</v>
       </c>
       <c r="D262" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E262" s="4" t="s">
         <v>110</v>
@@ -28125,7 +28152,7 @@
         <v>53</v>
       </c>
       <c r="D263" s="4">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E263" s="4" t="s">
         <v>110</v>
@@ -28147,7 +28174,7 @@
         <v>53</v>
       </c>
       <c r="D264" s="4">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E264" s="4" t="s">
         <v>110</v>
@@ -28169,7 +28196,7 @@
         <v>53</v>
       </c>
       <c r="D265" s="4">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E265" s="4" t="s">
         <v>110</v>
@@ -28191,7 +28218,7 @@
         <v>53</v>
       </c>
       <c r="D266" s="4">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E266" s="4" t="s">
         <v>110</v>
@@ -28213,7 +28240,7 @@
         <v>53</v>
       </c>
       <c r="D267" s="4">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E267" s="4" t="s">
         <v>110</v>
@@ -28235,7 +28262,7 @@
         <v>53</v>
       </c>
       <c r="D268" s="4">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E268" s="4" t="s">
         <v>110</v>
@@ -28257,7 +28284,7 @@
         <v>53</v>
       </c>
       <c r="D269" s="4">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E269" s="4" t="s">
         <v>110</v>
@@ -28279,7 +28306,7 @@
         <v>53</v>
       </c>
       <c r="D270" s="4">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E270" s="4" t="s">
         <v>110</v>
@@ -28301,7 +28328,7 @@
         <v>53</v>
       </c>
       <c r="D271" s="4">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E271" s="4" t="s">
         <v>110</v>
@@ -28323,7 +28350,7 @@
         <v>53</v>
       </c>
       <c r="D272" s="4">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E272" s="4" t="s">
         <v>110</v>
@@ -28345,7 +28372,7 @@
         <v>53</v>
       </c>
       <c r="D273" s="4">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E273" s="4" t="s">
         <v>110</v>
@@ -28367,7 +28394,7 @@
         <v>53</v>
       </c>
       <c r="D274" s="4">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E274" s="4" t="s">
         <v>110</v>
@@ -28389,7 +28416,7 @@
         <v>53</v>
       </c>
       <c r="D275" s="4">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E275" s="4" t="s">
         <v>110</v>
@@ -28411,7 +28438,7 @@
         <v>53</v>
       </c>
       <c r="D276" s="4">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E276" s="4" t="s">
         <v>110</v>
@@ -28433,7 +28460,7 @@
         <v>53</v>
       </c>
       <c r="D277" s="4">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E277" s="4" t="s">
         <v>110</v>
@@ -28455,7 +28482,7 @@
         <v>53</v>
       </c>
       <c r="D278" s="4">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E278" s="4" t="s">
         <v>110</v>
@@ -28477,7 +28504,7 @@
         <v>53</v>
       </c>
       <c r="D279" s="4">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E279" s="4" t="s">
         <v>110</v>
@@ -28499,16 +28526,16 @@
         <v>53</v>
       </c>
       <c r="D280" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E280" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F280" s="12">
-        <v>43206</v>
+        <v>43217</v>
       </c>
       <c r="G280" s="4" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="H280" s="4"/>
       <c r="I280" s="6"/>
@@ -28521,7 +28548,7 @@
         <v>53</v>
       </c>
       <c r="D281" s="4">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E281" s="4" t="s">
         <v>110</v>
@@ -28543,7 +28570,7 @@
         <v>53</v>
       </c>
       <c r="D282" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E282" s="4" t="s">
         <v>110</v>
@@ -28565,7 +28592,7 @@
         <v>53</v>
       </c>
       <c r="D283" s="4">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E283" s="4" t="s">
         <v>110</v>
@@ -28587,7 +28614,7 @@
         <v>53</v>
       </c>
       <c r="D284" s="4">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E284" s="4" t="s">
         <v>110</v>
@@ -28609,7 +28636,7 @@
         <v>53</v>
       </c>
       <c r="D285" s="4">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E285" s="4" t="s">
         <v>110</v>
@@ -28631,7 +28658,7 @@
         <v>53</v>
       </c>
       <c r="D286" s="4">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E286" s="4" t="s">
         <v>110</v>
@@ -28653,7 +28680,7 @@
         <v>53</v>
       </c>
       <c r="D287" s="4">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E287" s="4" t="s">
         <v>110</v>
@@ -28675,7 +28702,7 @@
         <v>53</v>
       </c>
       <c r="D288" s="4">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E288" s="4" t="s">
         <v>110</v>
@@ -28697,7 +28724,7 @@
         <v>53</v>
       </c>
       <c r="D289" s="4">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E289" s="4" t="s">
         <v>110</v>
@@ -28719,7 +28746,7 @@
         <v>53</v>
       </c>
       <c r="D290" s="4">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E290" s="4" t="s">
         <v>110</v>
@@ -28733,29 +28760,8 @@
       <c r="H290" s="4"/>
       <c r="I290" s="6"/>
     </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B291" s="12">
-        <v>43273</v>
-      </c>
-      <c r="C291" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D291" s="4">
-        <v>175</v>
-      </c>
-      <c r="E291" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F291" s="12">
-        <v>43217</v>
-      </c>
-      <c r="G291" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H291" s="4"/>
-      <c r="I291" s="6"/>
-    </row>
   </sheetData>
+  <autoFilter ref="B1:I290" xr:uid="{75C24F79-1AF7-4BAB-B925-57DAF3C9E38A}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rozdzial o I etapie szachownicy w trakcie
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D25081-F9F3-44FB-8456-D55AB710635C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5A0B94-C08B-4F31-AD58-83AB4E4E6286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeracja eksplantatów" sheetId="4" r:id="rId1"/>
@@ -923,10 +923,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1594,9 +1594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ159"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
@@ -1647,90 +1648,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17" t="s">
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17" t="s">
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17" t="s">
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17" t="s">
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17" t="s">
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="17"/>
-      <c r="AN1" s="17" t="s">
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="AO1" s="17"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="17"/>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="18"/>
+    </row>
+    <row r="2" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="3" t="s">
         <v>111</v>
       </c>
@@ -1840,7 +1841,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43168</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -2888,7 +2889,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -3019,7 +3020,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -3543,7 +3544,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -3674,7 +3675,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -3936,7 +3937,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -4198,7 +4199,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43175</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
@@ -4460,7 +4461,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -4722,7 +4723,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
@@ -4853,7 +4854,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>31</v>
       </c>
@@ -4984,7 +4985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -5246,7 +5247,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -5508,7 +5509,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
@@ -5639,7 +5640,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -5770,7 +5771,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -5901,7 +5902,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -6032,7 +6033,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
@@ -6294,7 +6295,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>31</v>
       </c>
@@ -6425,7 +6426,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>31</v>
       </c>
@@ -6556,7 +6557,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
@@ -6687,7 +6688,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
@@ -6818,7 +6819,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
@@ -6949,7 +6950,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>31</v>
       </c>
@@ -7080,7 +7081,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
@@ -7211,7 +7212,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>31</v>
       </c>
@@ -7342,7 +7343,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
@@ -7473,7 +7474,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>31</v>
       </c>
@@ -7604,7 +7605,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>31</v>
       </c>
@@ -7735,7 +7736,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>31</v>
       </c>
@@ -7866,7 +7867,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>31</v>
       </c>
@@ -7997,7 +7998,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
@@ -8128,7 +8129,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>31</v>
       </c>
@@ -8259,7 +8260,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
@@ -8390,7 +8391,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>31</v>
       </c>
@@ -8521,7 +8522,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>31</v>
       </c>
@@ -8652,7 +8653,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>31</v>
       </c>
@@ -8783,7 +8784,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>31</v>
       </c>
@@ -8914,7 +8915,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>43182</v>
       </c>
@@ -9045,7 +9046,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>50</v>
       </c>
@@ -9176,7 +9177,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>50</v>
       </c>
@@ -9307,7 +9308,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>50</v>
       </c>
@@ -9438,7 +9439,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>50</v>
       </c>
@@ -9569,7 +9570,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>50</v>
       </c>
@@ -9700,7 +9701,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>50</v>
       </c>
@@ -9831,7 +9832,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>50</v>
       </c>
@@ -9962,7 +9963,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>50</v>
       </c>
@@ -10093,7 +10094,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>50</v>
       </c>
@@ -10224,7 +10225,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>50</v>
       </c>
@@ -10355,7 +10356,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>50</v>
       </c>
@@ -10486,7 +10487,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>50</v>
       </c>
@@ -10617,7 +10618,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>50</v>
       </c>
@@ -10748,7 +10749,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>50</v>
       </c>
@@ -10879,7 +10880,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>50</v>
       </c>
@@ -11010,7 +11011,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>50</v>
       </c>
@@ -11141,7 +11142,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="74" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:43" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>50</v>
       </c>
@@ -11272,7 +11273,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>51</v>
       </c>
@@ -11403,7 +11404,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>43196</v>
       </c>
@@ -11534,7 +11535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>51</v>
       </c>
@@ -11665,7 +11666,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>51</v>
       </c>
@@ -11796,7 +11797,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>51</v>
       </c>
@@ -11927,7 +11928,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>51</v>
       </c>
@@ -12058,7 +12059,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>51</v>
       </c>
@@ -12189,7 +12190,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>51</v>
       </c>
@@ -12320,7 +12321,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>51</v>
       </c>
@@ -12451,7 +12452,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>51</v>
       </c>
@@ -12582,7 +12583,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>51</v>
       </c>
@@ -12713,7 +12714,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>51</v>
       </c>
@@ -12844,7 +12845,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>51</v>
       </c>
@@ -12975,7 +12976,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>51</v>
       </c>
@@ -13106,7 +13107,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>51</v>
       </c>
@@ -13237,7 +13238,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>51</v>
       </c>
@@ -13368,7 +13369,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>51</v>
       </c>
@@ -13499,7 +13500,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>43196</v>
       </c>
@@ -13630,7 +13631,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>43196</v>
       </c>
@@ -13761,7 +13762,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>52</v>
       </c>
@@ -13892,7 +13893,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>52</v>
       </c>
@@ -14023,7 +14024,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>52</v>
       </c>
@@ -14154,7 +14155,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>52</v>
       </c>
@@ -14285,7 +14286,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>80</v>
       </c>
@@ -14416,7 +14417,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>80</v>
       </c>
@@ -14547,7 +14548,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>80</v>
       </c>
@@ -22305,6 +22306,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AQ159" xr:uid="{A3EB1D5E-4AF2-4E96-A39F-D43A7CF18BB2}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Szachownica kostkowata"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
     <filterColumn colId="9" showButton="0"/>
@@ -22360,7 +22366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -22377,22 +22383,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>105</v>
       </c>
       <c r="H1" s="16" t="s">

</xml_diff>

<commit_message>
Dodanie informacji o publikacjach Fritillaria oraz tabelka ze sposiem ekspalntatow po pierwszy metapie
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5A0B94-C08B-4F31-AD58-83AB4E4E6286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6AC11E-1A5D-458B-95BC-9B4077EDBAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7268" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7260" uniqueCount="262">
   <si>
     <t>Data</t>
   </si>
@@ -1597,8 +1597,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14680,8 +14680,8 @@
       </c>
     </row>
     <row r="101" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>52</v>
+      <c r="A101" s="12">
+        <v>43206</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>53</v>
@@ -15196,8 +15196,8 @@
       </c>
     </row>
     <row r="105" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>52</v>
+      <c r="A105" s="12">
+        <v>43206</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>53</v>
@@ -17403,8 +17403,8 @@
       </c>
     </row>
     <row r="122" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
-        <v>81</v>
+      <c r="A122" s="12">
+        <v>43217</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>53</v>
@@ -18306,8 +18306,8 @@
       </c>
     </row>
     <row r="129" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
-        <v>81</v>
+      <c r="A129" s="12">
+        <v>43217</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>53</v>
@@ -18693,8 +18693,8 @@
       </c>
     </row>
     <row r="132" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>81</v>
+      <c r="A132" s="12">
+        <v>43217</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>53</v>
@@ -19725,8 +19725,8 @@
       </c>
     </row>
     <row r="140" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A140" s="4" t="s">
-        <v>92</v>
+      <c r="A140" s="12">
+        <v>43231</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>53</v>
@@ -20757,8 +20757,8 @@
       </c>
     </row>
     <row r="148" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A148" s="4" t="s">
-        <v>92</v>
+      <c r="A148" s="12">
+        <v>43231</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>53</v>
@@ -21015,8 +21015,8 @@
       </c>
     </row>
     <row r="150" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A150" s="4" t="s">
-        <v>92</v>
+      <c r="A150" s="12">
+        <v>43231</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Organogenza korzeniowa - rozdzial
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BE50FD-45FF-4FC6-AF20-E1C486D3B33B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58CC8A2-D032-4F3F-9AFC-3383AEABCF6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3840" yWindow="4665" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeracja eksplantatów" sheetId="4" r:id="rId1"/>
@@ -1609,8 +1609,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ163"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AH99" sqref="AH99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,7 +1853,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43168</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43175</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>31</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>31</v>
       </c>
@@ -6438,7 +6438,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>31</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>31</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>31</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>31</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>31</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>31</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>31</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>31</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>31</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>31</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>31</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>31</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>43182</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>50</v>
       </c>
@@ -9189,7 +9189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>50</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>50</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>50</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>50</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>50</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>50</v>
       </c>
@@ -9975,7 +9975,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>50</v>
       </c>
@@ -10106,7 +10106,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>50</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>50</v>
       </c>
@@ -10368,7 +10368,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>50</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>50</v>
       </c>
@@ -10630,7 +10630,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>50</v>
       </c>
@@ -10761,7 +10761,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>50</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>50</v>
       </c>
@@ -11023,7 +11023,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="73" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>50</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="74" spans="1:43" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>50</v>
       </c>
@@ -11285,7 +11285,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="75" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>51</v>
       </c>
@@ -11416,7 +11416,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>43196</v>
       </c>
@@ -11547,7 +11547,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>51</v>
       </c>
@@ -11678,7 +11678,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="78" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>51</v>
       </c>
@@ -11809,7 +11809,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>51</v>
       </c>
@@ -11940,7 +11940,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>51</v>
       </c>
@@ -12071,7 +12071,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>51</v>
       </c>
@@ -12202,7 +12202,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>51</v>
       </c>
@@ -12333,7 +12333,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>51</v>
       </c>
@@ -12464,7 +12464,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>51</v>
       </c>
@@ -12595,7 +12595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>51</v>
       </c>
@@ -12726,7 +12726,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>51</v>
       </c>
@@ -12857,7 +12857,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>51</v>
       </c>
@@ -12988,7 +12988,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>51</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>51</v>
       </c>
@@ -13250,7 +13250,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>51</v>
       </c>
@@ -13381,7 +13381,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>51</v>
       </c>
@@ -13512,7 +13512,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>43196</v>
       </c>
@@ -13643,7 +13643,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="93" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>43196</v>
       </c>
@@ -13774,7 +13774,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>52</v>
       </c>
@@ -13905,7 +13905,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>52</v>
       </c>
@@ -14036,7 +14036,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>52</v>
       </c>
@@ -14167,7 +14167,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>52</v>
       </c>
@@ -14298,7 +14298,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>80</v>
       </c>
@@ -14429,7 +14429,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>80</v>
       </c>
@@ -14560,7 +14560,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>80</v>
       </c>
@@ -14691,7 +14691,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12">
         <v>43161</v>
       </c>
@@ -14748,7 +14748,7 @@
       <c r="AP101" s="4"/>
       <c r="AQ101" s="4"/>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>43161</v>
       </c>
@@ -14805,7 +14805,7 @@
       <c r="AP102" s="4"/>
       <c r="AQ102" s="4"/>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12">
         <v>43161</v>
       </c>
@@ -14862,7 +14862,7 @@
       <c r="AP103" s="4"/>
       <c r="AQ103" s="4"/>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12">
         <v>43161</v>
       </c>
@@ -14919,7 +14919,7 @@
       <c r="AP104" s="4"/>
       <c r="AQ104" s="4"/>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12">
         <v>43206</v>
       </c>
@@ -15048,7 +15048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>52</v>
       </c>
@@ -15177,7 +15177,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>52</v>
       </c>
@@ -15306,7 +15306,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>52</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12">
         <v>43206</v>
       </c>
@@ -15564,7 +15564,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>52</v>
       </c>
@@ -15693,7 +15693,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>52</v>
       </c>
@@ -15822,7 +15822,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>52</v>
       </c>
@@ -15951,7 +15951,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>52</v>
       </c>
@@ -16080,7 +16080,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>52</v>
       </c>
@@ -16209,7 +16209,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>52</v>
       </c>
@@ -16338,7 +16338,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>52</v>
       </c>
@@ -16467,7 +16467,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>52</v>
       </c>
@@ -16596,7 +16596,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>52</v>
       </c>
@@ -16725,7 +16725,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>52</v>
       </c>
@@ -16856,7 +16856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>52</v>
       </c>
@@ -16987,7 +16987,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>52</v>
       </c>
@@ -17118,7 +17118,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>52</v>
       </c>
@@ -17249,7 +17249,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>52</v>
       </c>
@@ -17380,7 +17380,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>52</v>
       </c>
@@ -17511,7 +17511,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>52</v>
       </c>
@@ -17642,7 +17642,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12">
         <v>43217</v>
       </c>
@@ -17771,7 +17771,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>81</v>
       </c>
@@ -17900,7 +17900,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>81</v>
       </c>
@@ -18029,7 +18029,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>81</v>
       </c>
@@ -18158,7 +18158,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>81</v>
       </c>
@@ -18287,7 +18287,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>81</v>
       </c>
@@ -18416,7 +18416,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>81</v>
       </c>
@@ -18545,7 +18545,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12">
         <v>43217</v>
       </c>
@@ -18674,7 +18674,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -18803,7 +18803,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>81</v>
       </c>
@@ -18932,7 +18932,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12">
         <v>43217</v>
       </c>
@@ -19061,7 +19061,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>81</v>
       </c>
@@ -19190,7 +19190,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>81</v>
       </c>
@@ -19319,7 +19319,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>81</v>
       </c>
@@ -19448,7 +19448,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>81</v>
       </c>
@@ -19577,7 +19577,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>81</v>
       </c>
@@ -19706,7 +19706,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>81</v>
       </c>
@@ -19835,7 +19835,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>81</v>
       </c>
@@ -19964,7 +19964,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12">
         <v>43231</v>
       </c>
@@ -20093,7 +20093,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>92</v>
       </c>
@@ -20222,7 +20222,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>92</v>
       </c>
@@ -20351,7 +20351,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>92</v>
       </c>
@@ -20480,7 +20480,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>92</v>
       </c>
@@ -20609,7 +20609,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>92</v>
       </c>
@@ -20738,7 +20738,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>92</v>
       </c>
@@ -20867,7 +20867,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>92</v>
       </c>
@@ -20996,7 +20996,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12">
         <v>43231</v>
       </c>
@@ -21125,7 +21125,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>92</v>
       </c>
@@ -21254,7 +21254,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12">
         <v>43231</v>
       </c>
@@ -21383,7 +21383,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>92</v>
       </c>
@@ -21512,7 +21512,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>92</v>
       </c>
@@ -21641,7 +21641,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>92</v>
       </c>
@@ -21770,7 +21770,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="158" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>92</v>
       </c>
@@ -21899,7 +21899,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="159" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>92</v>
       </c>
@@ -22028,7 +22028,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="160" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>92</v>
       </c>
@@ -22157,7 +22157,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="161" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>92</v>
       </c>
@@ -22286,7 +22286,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="162" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>92</v>
       </c>
@@ -22415,7 +22415,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="163" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>92</v>
       </c>
@@ -22548,7 +22548,7 @@
   <autoFilter ref="A1:AQ163" xr:uid="{A3EB1D5E-4AF2-4E96-A39F-D43A7CF18BB2}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Szachownica kostkowata"/>
+        <filter val="Snieżyca karpacka"/>
       </filters>
     </filterColumn>
     <filterColumn colId="7" showButton="0"/>
@@ -22606,7 +22606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Wszsytko poza rozdzialem o badaniu zywotnosci plku
</commit_message>
<xml_diff>
--- a/Spisane eskplantaty.xlsx
+++ b/Spisane eskplantaty.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58CC8A2-D032-4F3F-9AFC-3383AEABCF6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C8343-F179-4FE7-9FB7-21D5FA1F939E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3840" yWindow="4665" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeracja eksplantatów" sheetId="4" r:id="rId1"/>
@@ -1609,7 +1609,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A90" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="AH99" sqref="AH99"/>
     </sheetView>
   </sheetViews>
@@ -22606,8 +22606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I346"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>